<commit_message>
Eintragung zweier Tätigkeiten bei Julian
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jules\Desktop\HTL\Diplomarbeit\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jules\Desktop\HTL\Diplomarbeit\Project\Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6EA716-A18F-4A0F-A1D2-576E5FA8B788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB8E227-9E33-49E2-B582-AF7661967827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{049A7F7D-90D2-44D3-8CB1-77B0E769D8E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Maxi</t>
   </si>
@@ -54,6 +54,19 @@
   </si>
   <si>
     <t>Datum</t>
+  </si>
+  <si>
+    <t>15.04.2022</t>
+  </si>
+  <si>
+    <t>Diskussion und Auswahl 
+der verwendeten Technologien</t>
+  </si>
+  <si>
+    <t>26.06.2022</t>
+  </si>
+  <si>
+    <t>Erstellen einer Projektumfangsdefinition</t>
   </si>
 </sst>
 </file>
@@ -92,14 +105,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,20 +437,21 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -448,10 +468,10 @@
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1">
         <f>SUM(C3)</f>
         <v>0</v>
@@ -469,23 +489,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3231478B-2541-4A9B-8D80-73344FCE226A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -498,23 +519,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1">
-        <f>SUM(C3)</f>
-        <v>0</v>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1">
+        <f>SUM(C3:C4)</f>
+        <v>2.8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hinzufügen von Resourcen und Update der Zeiterfassung
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jules\Desktop\HTL\Diplomarbeit\Project\Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB50AC0C-F0CA-46C9-9425-963F0A569146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60422A99-9E84-4319-8EC4-2027B961B28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{049A7F7D-90D2-44D3-8CB1-77B0E769D8E7}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{049A7F7D-90D2-44D3-8CB1-77B0E769D8E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Maxi" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Maxi</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Erstellen einer Projektumfangsdefinition</t>
+  </si>
+  <si>
+    <t>03.07.2022</t>
+  </si>
+  <si>
+    <t>Frontend Design Login- und Landing-Page</t>
   </si>
 </sst>
 </file>
@@ -114,14 +120,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FB1B17-6B24-40B8-9750-7982E255D2E4}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -450,11 +456,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -474,15 +480,15 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1">
         <f>SUM(C3)</f>
         <v>1.5</v>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3231478B-2541-4A9B-8D80-73344FCE226A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,11 +519,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -552,20 +558,31 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="1">
-        <f>SUM(C3:C4)</f>
-        <v>2.8</v>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1">
+        <f>SUM(C3:C5)</f>
+        <v>4.1999999999999993</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>